<commit_message>
pie chart - venue topic
</commit_message>
<xml_diff>
--- a/primary study.xlsx
+++ b/primary study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/XR-testing-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC75EB2-8076-3444-81A0-089B7FF757AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB9A663-9848-F148-B8DB-B6027C0A05FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="3160" windowWidth="28040" windowHeight="17440" xr2:uid="{ED65C1BC-2362-384C-95A2-151E4AED2308}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26540" xr2:uid="{ED65C1BC-2362-384C-95A2-151E4AED2308}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="91">
   <si>
     <t>doi</t>
   </si>
@@ -272,14 +272,50 @@
     <t>ACM International Conference on the Foundations of Software Engineering (FSE)</t>
   </si>
   <si>
+    <t>https://doi.org/10.1109/vr46266.2020.00013</t>
+  </si>
+  <si>
+    <t>ARCHIE: A User-Focused Framework for Testing Augmented Reality Applications in the Wild</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/uemcon47517.2019.8992974</t>
+  </si>
+  <si>
+    <t>Quality Model for Testing Augmented Reality Applications</t>
+  </si>
+  <si>
+    <t>duplicated</t>
+  </si>
+  <si>
+    <t>IEEE Conference on Virtual Reality and 3D User Interfaces (VR)</t>
+  </si>
+  <si>
+    <t>IEEE Annual Ubiquitous Computing, Electronics &amp; Mobile Communication Conference (UEMCON)</t>
+  </si>
+  <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Venue Topic</t>
+  </si>
+  <si>
+    <t>HCI</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Testing / Engineering</t>
+  </si>
+  <si>
+    <t>XR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,6 +350,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -336,12 +379,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -677,488 +721,693 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE58F1D-75DC-5A49-8CFE-42CF961AF14C}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="90.5" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="67.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="5" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="67.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
         <v>2019</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>2017</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
         <v>2018</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
         <v>2003</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2019</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
         <v>2019</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
         <v>2019</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
         <v>2022</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
         <v>2022</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
         <v>2023</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
         <v>2008</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
         <v>2020</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
         <v>2020</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
         <v>2020</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
         <v>2011</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
         <v>2023</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
         <v>2020</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
         <v>2021</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
         <v>2023</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
         <v>2023</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
         <v>2023</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
         <v>2023</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
         <v>2019</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
         <v>2019</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
         <v>2022</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
         <v>2024</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{35FA0E15-88A8-8547-9320-A97E1EC5E674}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{A55A7F83-14AF-A54A-AF71-00919B18104B}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{5D120FC6-5B1A-E549-ABF3-21DC3651A0FD}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{2B005949-C42E-6D4E-911F-AD9797FB124F}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{F315D919-1716-0B4A-A1FC-3CA8EA12F88A}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{90E802B4-D971-3D49-8AC6-EEEF0F58C73D}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{21B48D3A-6C5B-F84C-97BC-2A8EB14E2EDB}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{E631D09F-CAB4-AA4B-A294-FD3A072F7DD1}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{3822988D-73BA-AB43-8A2B-9BF5230B00A9}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{995FDFF0-857A-F141-A77A-BE341CB2D7DA}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{5248BC15-8D33-A044-9703-3EC73217230A}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{E676FE70-5AEC-C34F-88C4-26D23A0C1A76}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{C9E6E012-2B9B-2A44-BBA5-A98090E2EE60}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{77CB47D4-2808-8345-A71F-95A817167E37}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{5D55E53C-F801-5A46-B3E4-073F78EAB702}"/>
-    <hyperlink ref="A17" r:id="rId16" xr:uid="{3911FBC1-E8B8-914C-9122-6FC0630940C4}"/>
-    <hyperlink ref="A18" r:id="rId17" xr:uid="{BA552B9B-70E9-974E-890E-799294E1C5C1}"/>
-    <hyperlink ref="A19" r:id="rId18" xr:uid="{8E8DF64C-D596-5C48-BC92-17655595EA72}"/>
-    <hyperlink ref="A20" r:id="rId19" xr:uid="{BE38412C-A0FF-D64B-801B-93C395FE70A3}"/>
-    <hyperlink ref="A21" r:id="rId20" xr:uid="{E1886730-9963-0845-A926-5EE3561AC19E}"/>
-    <hyperlink ref="A22" r:id="rId21" xr:uid="{E415D3F9-0B23-464E-AC36-B0CFDB95257D}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{9DA522B7-692A-D94E-9063-9A962A073C00}"/>
-    <hyperlink ref="A24" r:id="rId23" xr:uid="{B71E7847-F836-FB49-9CEB-BB08B94E80A8}"/>
-    <hyperlink ref="A25" r:id="rId24" xr:uid="{2EDF2B47-DFAA-3049-BBF3-4E6C4002AEC6}"/>
-    <hyperlink ref="A26" r:id="rId25" xr:uid="{1C78D0FC-8451-DB43-8F43-4AF13956892A}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F98C1AA0-8951-D347-8631-BDBDD841348B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{38CE04AB-DA05-5947-A5C2-536DD2A93500}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{02C5ED2E-A38B-524F-B41F-D3D82C8AD776}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{85ADA27B-2D2E-9543-9913-FDC4F4EB90B9}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{742959D2-3E20-E64B-9DA1-7702DD6BD414}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{39CE488A-0078-D54D-B435-B30DE60BE519}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{5710565A-FF18-A744-B05D-63619853E297}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{FF13E537-21CB-A343-96F9-706C88432039}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{BBAD4E60-784C-D947-9D12-7858F3638E8F}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{92C89044-E9F7-6843-8B95-2258088605CD}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{2C1998E4-A636-BF4E-BFD4-6A63A8387C4D}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{E9DF4411-1722-FD4D-AF79-AA541A16BB8D}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{8D56FC67-C7CA-3146-B9FA-AFB5C7F6774B}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{1C8B1A9B-DCC6-E544-B22D-2355F72F687D}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{29EE39A9-7ABB-5149-A33A-AF4932427E43}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{5BDEBC5D-FF25-F141-8ABC-48594E5387B4}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{D5FDCF9E-0DF6-2F41-BC43-EC07E7DD504C}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{3B9396BA-4F8A-E341-8C9F-A97E021F1690}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{93D55F35-4214-1C40-9516-32A722FC75E5}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{970DF260-4574-7848-8A93-C4AF97D6A4B0}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{5DA4B3E4-04F4-8A43-9528-FB70D22E75C7}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{9D25BD95-D927-C94B-8018-1C69E50A2621}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{0E1E569A-7CF3-3A4C-BE9F-AF4F0F20ACB0}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{FD6A4F7A-DCB1-1942-AC63-C8D1C7FCD4C8}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{CB03EB7F-3D44-2647-89B3-BB1DC64BE514}"/>
+    <hyperlink ref="A27" r:id="rId26" xr:uid="{4572608A-C6DF-644D-B722-871133D47DA0}"/>
+    <hyperlink ref="A28" r:id="rId27" xr:uid="{33EBF006-5FF9-2340-83B0-2162C2318E3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>